<commit_message>
4.3 - 4.3.1 Modificando o capitulo de casos de teste
</commit_message>
<xml_diff>
--- a/resultados da roteirização.xlsx
+++ b/resultados da roteirização.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18345" windowHeight="7815"/>
+    <workbookView windowWidth="20385" windowHeight="8355" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="tatalização" sheetId="1" r:id="rId1"/>
+    <sheet name="separadas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19">
   <si>
     <t>Resultado Roteirização - Tempo</t>
   </si>
@@ -56,6 +57,21 @@
   </si>
   <si>
     <t>Distância SysRLog</t>
+  </si>
+  <si>
+    <t>Resultado Roteirização - Caso de Teste 1 - Cidade de Caçapava</t>
+  </si>
+  <si>
+    <t>Valor obtido GoogleMaps</t>
+  </si>
+  <si>
+    <t>Valor Obtido SysRLog</t>
+  </si>
+  <si>
+    <t>Tempo(horas)</t>
+  </si>
+  <si>
+    <t>Distância(KMs)</t>
   </si>
 </sst>
 </file>
@@ -63,10 +79,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -85,6 +101,83 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -94,7 +187,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -114,8 +221,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -131,101 +239,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -250,49 +266,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -304,103 +422,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -410,32 +450,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -444,6 +460,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color theme="0"/>
@@ -527,6 +558,63 @@
       </top>
       <bottom style="thin">
         <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -546,30 +634,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -585,21 +649,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -610,215 +659,212 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1142,8 +1188,8 @@
   <sheetPr/>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:E15"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="4"/>
@@ -1153,246 +1199,250 @@
     <col min="3" max="3" width="16.4285714285714" customWidth="1"/>
     <col min="4" max="4" width="9.14285714285714" customWidth="1"/>
     <col min="5" max="5" width="19.1428571428571" customWidth="1"/>
+    <col min="8" max="8" width="23" customWidth="1"/>
+    <col min="9" max="9" width="20.7142857142857" customWidth="1"/>
+    <col min="10" max="10" width="18.2857142857143" customWidth="1"/>
+    <col min="12" max="12" width="21.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" ht="13.5" spans="1:5">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="10">
         <v>0.0368055555555556</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="10">
         <v>0.0284722222222222</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="11">
         <f>B3-C3</f>
         <v>0.00833333333333333</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="12">
         <f>D3/B3</f>
         <v>0.226415094339623</v>
       </c>
     </row>
-    <row r="4" ht="14.25" spans="1:5">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:5">
+      <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="10">
         <v>0.0729166666666667</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="10">
         <v>0.0486111111111111</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="11">
         <f>B4-C4</f>
         <v>0.0243055555555556</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="12">
         <f>D4/B4</f>
         <v>0.333333333333333</v>
       </c>
     </row>
-    <row r="5" ht="14.25" spans="1:5">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="10">
         <v>0.0791666666666667</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="10">
         <v>0.0534722222222222</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="11">
         <f>B5-C5</f>
         <v>0.0256944444444444</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="12">
         <f>D5/B5</f>
         <v>0.324561403508772</v>
       </c>
     </row>
-    <row r="6" ht="14.25" spans="1:5">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="10">
         <v>0.0694444444444444</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="10">
         <v>0.0430555555555556</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="11">
         <f>B6-C6</f>
         <v>0.0263888888888889</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="12">
         <f>D6/B6</f>
         <v>0.38</v>
       </c>
     </row>
-    <row r="7" ht="13.5" spans="1:5">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:5">
+      <c r="A7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="14">
         <v>0.03125</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="14">
         <v>0.0270833333333333</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="11">
         <f>B7-C7</f>
         <v>0.00416666666666667</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="12">
         <f>D7/B7</f>
         <v>0.133333333333333</v>
       </c>
     </row>
     <row r="9" ht="13.5" spans="1:5">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="14.25" spans="1:5">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" ht="14.25" spans="1:5">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="15">
         <v>21.4</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="15">
         <v>16.4</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="16">
         <f>B11-C11</f>
         <v>5</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="17">
         <f>D11/B11</f>
         <v>0.233644859813084</v>
       </c>
     </row>
     <row r="12" ht="14.25" spans="1:5">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="15">
         <v>65.9</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="15">
         <v>37.3</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="16">
         <f>B12-C12</f>
         <v>28.6</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="17">
         <f>D12/B12</f>
         <v>0.433990895295903</v>
       </c>
     </row>
     <row r="13" ht="14.25" spans="1:5">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="15">
         <v>66.3</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="15">
         <v>37.8</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="16">
         <f>B13-C13</f>
         <v>28.5</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="17">
         <f>D13/B13</f>
         <v>0.429864253393665</v>
       </c>
     </row>
     <row r="14" ht="14.25" spans="1:5">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="15">
         <v>51.2</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="15">
         <v>35.1</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="16">
         <f>B14-C14</f>
         <v>16.1</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="17">
         <f>D14/B14</f>
         <v>0.314453125</v>
       </c>
     </row>
     <row r="15" ht="13.5" spans="1:5">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="18">
         <v>23.1</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="18">
         <v>18.6</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="16">
         <f>B15-C15</f>
         <v>4.5</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="17">
         <f>D15/B15</f>
         <v>0.194805194805195</v>
       </c>
@@ -1405,4 +1455,88 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="B2:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B2:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="4" outlineLevelCol="5"/>
+  <cols>
+    <col min="2" max="2" width="14.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="12.2857142857143" customWidth="1"/>
+    <col min="4" max="4" width="10.8571428571429" customWidth="1"/>
+    <col min="6" max="6" width="10.4285714285714" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6">
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" s="1" customFormat="1" ht="25.5" spans="2:6">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.0368055555555556</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.0284722222222222</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.00833333333333333</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0.226415094339623</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4">
+        <v>21.4</v>
+      </c>
+      <c r="D5" s="4">
+        <v>16.4</v>
+      </c>
+      <c r="E5" s="4">
+        <v>5</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.233644859813084</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:F2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Efetuada as correcoes basicas pontuadas pelo Mineda|Efetuada alteracoes documentos da apresentacao
</commit_message>
<xml_diff>
--- a/resultados da roteirização.xlsx
+++ b/resultados da roteirização.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="13035" activeTab="5"/>
+    <workbookView windowWidth="17625" windowHeight="10155" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="tatalização" sheetId="1" r:id="rId1"/>
@@ -98,10 +98,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -120,10 +120,94 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -135,37 +219,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -174,14 +227,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -190,16 +235,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -207,43 +251,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -256,13 +263,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -285,25 +285,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -315,157 +447,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -618,17 +618,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -637,7 +633,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -666,26 +662,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -697,6 +673,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -720,152 +720,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -896,6 +896,9 @@
     <xf numFmtId="10" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -911,14 +914,8 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1268,7 +1265,7 @@
   <sheetPr/>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15:E15"/>
     </sheetView>
   </sheetViews>
@@ -1286,160 +1283,160 @@
   </cols>
   <sheetData>
     <row r="1" ht="13.5" spans="1:5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
     </row>
     <row r="2" ht="13.5" spans="1:5">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="20">
         <v>0.0368055555555556</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="20">
         <v>0.0284722222222222</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="21">
         <f>B3-C3</f>
         <v>0.00833333333333333</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="22">
         <f>D3/B3</f>
         <v>0.226415094339623</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="20">
         <v>0.075</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="20">
         <v>0.0611111111111111</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="21">
         <f>B4-C4</f>
         <v>0.0138888888888889</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="22">
         <f>D4/B4</f>
         <v>0.185185185185185</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="20">
         <v>0.0805555555555556</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="20">
         <v>0.0506944444444444</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="21">
         <f>B5-C5</f>
         <v>0.0298611111111111</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="22">
         <f>D5/B5</f>
         <v>0.370689655172414</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="20">
         <v>0.0694444444444444</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="20">
         <v>0.0430555555555556</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="21">
         <f>B6-C6</f>
         <v>0.0263888888888889</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="22">
         <f>D6/B6</f>
         <v>0.38</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="24">
         <v>0.03125</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="24">
         <v>0.0270833333333333</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="21">
         <f>B7-C7</f>
         <v>0.00416666666666667</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="22">
         <f>D7/B7</f>
         <v>0.133333333333333</v>
       </c>
     </row>
     <row r="9" ht="13.5" spans="1:5">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
     </row>
     <row r="10" ht="14.25" spans="1:5">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" ht="14.25" spans="1:5">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="26">
+      <c r="B11" s="25">
         <v>21.4</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="25">
         <v>16.4</v>
       </c>
       <c r="D11" s="8">
@@ -1452,13 +1449,13 @@
       </c>
     </row>
     <row r="12" ht="14.25" spans="1:5">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="26">
+      <c r="B12" s="25">
         <v>68.1</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="25">
         <v>46.9</v>
       </c>
       <c r="D12" s="8">
@@ -1471,13 +1468,13 @@
       </c>
     </row>
     <row r="13" ht="14.25" spans="1:5">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="26">
+      <c r="B13" s="25">
         <v>58</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="25">
         <v>36</v>
       </c>
       <c r="D13" s="8">
@@ -1490,13 +1487,13 @@
       </c>
     </row>
     <row r="14" ht="14.25" spans="1:5">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="26">
+      <c r="B14" s="25">
         <v>51.2</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="25">
         <v>35.1</v>
       </c>
       <c r="D14" s="8">
@@ -1509,7 +1506,7 @@
       </c>
     </row>
     <row r="15" ht="13.5" spans="1:5">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="23" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="7">
@@ -1555,13 +1552,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" s="16" customFormat="1" ht="25.5" spans="2:6">
       <c r="B3" s="2"/>
@@ -1582,16 +1579,16 @@
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="15">
         <v>0.0368055555555556</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="15">
         <v>0.0284722222222222</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="15">
         <v>0.00833333333333333</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="10">
         <v>0.226415094339623</v>
       </c>
     </row>
@@ -1608,7 +1605,7 @@
       <c r="E5" s="3">
         <v>5</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="10">
         <v>0.233644859813084</v>
       </c>
     </row>
@@ -1627,7 +1624,7 @@
   <dimension ref="B2:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="4" outlineLevelCol="5"/>
@@ -1639,13 +1636,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" ht="30" customHeight="1" spans="2:6">
       <c r="B3" s="2"/>
@@ -1669,13 +1666,13 @@
       <c r="C4" s="4">
         <v>0.075</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="15">
         <v>0.0611111111111111</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="15">
         <v>0.0138888888888889</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="10">
         <v>0.185185185185185</v>
       </c>
     </row>
@@ -1692,7 +1689,7 @@
       <c r="E5" s="3">
         <v>21.2</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="10">
         <v>0.311306901615272</v>
       </c>
     </row>
@@ -1710,8 +1707,8 @@
   <sheetPr/>
   <dimension ref="B3:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="B3:F6"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="5" outlineLevelCol="5"/>
@@ -1723,13 +1720,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:6">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="13"/>
     </row>
     <row r="4" ht="29" customHeight="1" spans="2:6">
       <c r="B4" s="2"/>
@@ -1759,7 +1756,7 @@
       <c r="E5">
         <v>22</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="10">
         <v>0.379310344827586</v>
       </c>
     </row>
@@ -1767,16 +1764,16 @@
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="14">
         <v>0.0805555555555556</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="14">
         <v>0.0506944444444444</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="14">
         <v>0.0298611111111111</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="10">
         <v>0.370689655172414</v>
       </c>
     </row>
@@ -1794,8 +1791,8 @@
   <sheetPr/>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="4" outlineLevelCol="5"/>
@@ -1849,7 +1846,7 @@
       <c r="E4" s="6">
         <v>16.1</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="10">
         <v>0.314453125</v>
       </c>
     </row>
@@ -1866,7 +1863,7 @@
       <c r="E5" s="4">
         <v>0.0263888888888889</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="10">
         <v>0.38</v>
       </c>
     </row>
@@ -1884,8 +1881,8 @@
   <sheetPr/>
   <dimension ref="B2:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="6"/>
@@ -1955,6 +1952,7 @@
         <v>0.194805194805195</v>
       </c>
     </row>
+    <row r="8" ht="13.5"/>
     <row r="9" ht="13.5" spans="4:7">
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>

</xml_diff>